<commit_message>
Introduced the create a transaction button in the dashboard
</commit_message>
<xml_diff>
--- a/uploads/blank_excel_file.xlsx
+++ b/uploads/blank_excel_file.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD45486-FB2A-4C8E-B3A5-993BE361680C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -42,12 +43,15 @@
   </si>
   <si>
     <t>roll</t>
+  </si>
+  <si>
+    <t>class_numeric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,7 +126,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -130,6 +134,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -419,25 +426,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" customWidth="1"/>
+    <col min="6" max="6" width="28.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,12 +467,15 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="F3" s="2"/>
     </row>
@@ -479,12 +490,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -496,12 +507,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>